<commit_message>
Update Capstone_Quadcopter_Bill of Materials.xlsx
</commit_message>
<xml_diff>
--- a/Quad_Copter/Capstone_Quadcopter_Bill of Materials.xlsx
+++ b/Quad_Copter/Capstone_Quadcopter_Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/447eb0fe645bf98e/Documents/GitHub/Capstone-Sightline/Quad_Copter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{609E7FEF-C1FB-4D7F-AED1-D956BEC64491}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{1D8F7342-79A9-4B8D-9733-75B5581CAAC1}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{609E7FEF-C1FB-4D7F-AED1-D956BEC64491}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{39E51885-EEEB-489C-9902-1348132F97DE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,10 +166,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -493,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -545,6 +546,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,12 +593,8 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -910,7 +914,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -930,57 +934,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="27" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="42">
+      <c r="B3" s="42"/>
+      <c r="C3" s="45">
         <v>43480</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="1" t="s">
@@ -1288,13 +1292,13 @@
       <c r="F12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="22">
         <v>15</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="46">
         <v>39.950000000000003</v>
       </c>
       <c r="J12" s="9">
@@ -1307,7 +1311,7 @@
     </row>
     <row r="13" spans="1:11" ht="14.25" customHeight="1">
       <c r="A13" t="str">
-        <f t="shared" ref="A12:A360" si="1">IF(ISBLANK(C13),"",ROW()-4)</f>
+        <f t="shared" ref="A13:A360" si="1">IF(ISBLANK(C13),"",ROW()-4)</f>
         <v/>
       </c>
       <c r="B13" s="4"/>
@@ -1354,10 +1358,10 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="45">
+      <c r="H16" s="29">
         <f>SUM(H5:H12)</f>
         <v>1365.1999999999998</v>
       </c>

</xml_diff>